<commit_message>
code auto regiondebut compil
</commit_message>
<xml_diff>
--- a/Delphine/BDPT/Solutions/Solutions.xlsx
+++ b/Delphine/BDPT/Solutions/Solutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Solutec\GithuB\BDepBDD\Delphine\BDPT\Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C73E300-12B5-435B-B923-034EBFE93BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFFEC2F-9F80-4099-BD98-30A568255003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Identifier la région et la typologie</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>Remplacement du code</t>
+  </si>
+  <si>
+    <t>Remplacement code</t>
+  </si>
+  <si>
+    <t>Compil finale</t>
+  </si>
+  <si>
+    <t>Région</t>
   </si>
 </sst>
 </file>
@@ -751,8 +760,8 @@
   <sheetPr codeName="Feuil1" filterMode="1"/>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,50 +1140,63 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA9EC38-04CA-415F-B6A6-7CB0CABC86F5}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>